<commit_message>
Cambio de plantilla exportacion execel de aperturas
</commit_message>
<xml_diff>
--- a/Web/SPSA.Autorizadores/SPSA.Autorizadores.Web/Plantillas_Tablas/Plantilla_Aperturas/Platilla_DIRECTORIO-TIENDA-MASS.xlsx
+++ b/Web/SPSA.Autorizadores/SPSA.Autorizadores.Web/Plantillas_Tablas/Plantilla_Aperturas/Platilla_DIRECTORIO-TIENDA-MASS.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waly_\source\repositorios\Supermercados\sistema-autorizadores\Web\SPSA.Autorizadores\SPSA.Autorizadores.Web\Plantillas_Tablas\Plantilla_Aperturas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542A7659-F5CB-41C6-A18B-35092066FBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BCEF6F-5C8F-448D-9761-0C014945591C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="10095" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AA$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
   <si>
     <t>N°</t>
   </si>
@@ -108,9 +108,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>ACTIVA</t>
-  </si>
-  <si>
     <t>SurcoViejoSC MS</t>
   </si>
   <si>
@@ -172,6 +169,51 @@
   </si>
   <si>
     <t>MAE2</t>
+  </si>
+  <si>
+    <t>APERTURADO</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>ELIMINADO</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Codigo Sunat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Codigo EAN</t>
+  </si>
+  <si>
+    <t>Centro Distribucio</t>
+  </si>
+  <si>
+    <t>Tienda Espejo</t>
+  </si>
+  <si>
+    <t>Mt2 Sala</t>
+  </si>
+  <si>
+    <t>Zona Princing</t>
+  </si>
+  <si>
+    <t>Geolocalizacion</t>
+  </si>
+  <si>
+    <t>Fecha de Cierre</t>
+  </si>
+  <si>
+    <t>Numero de Guias</t>
+  </si>
+  <si>
+    <t>Spaceman (Modelo)</t>
   </si>
 </sst>
 </file>
@@ -259,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -302,12 +344,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -352,6 +422,10 @@
     <xf numFmtId="14" fontId="7" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -771,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,10 +868,19 @@
     <col min="14" max="14" width="18" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" customWidth="1"/>
     <col min="16" max="16" width="14.7109375" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="18" max="19" width="13.85546875" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" customWidth="1"/>
+    <col min="22" max="22" width="16" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" customWidth="1"/>
+    <col min="24" max="24" width="20.85546875" customWidth="1"/>
+    <col min="25" max="25" width="13.28515625" customWidth="1"/>
+    <col min="26" max="26" width="17.85546875" customWidth="1"/>
+    <col min="27" max="27" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -849,8 +932,38 @@
       <c r="Q1" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -897,31 +1010,43 @@
       <c r="P2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="13" t="s">
-        <v>26</v>
+      <c r="Q2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="14">
+        <v>44034</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="D3" s="9">
         <v>993548409</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>22</v>
@@ -931,10 +1056,10 @@
         <v>240</v>
       </c>
       <c r="K3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="M3" s="9">
         <v>1037481</v>
@@ -946,33 +1071,45 @@
         <v>42221</v>
       </c>
       <c r="P3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>26</v>
+        <v>51</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="14">
+        <v>44048</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>35</v>
       </c>
       <c r="D4" s="9">
         <v>993548463</v>
       </c>
       <c r="E4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>22</v>
@@ -982,10 +1119,10 @@
         <v>242</v>
       </c>
       <c r="K4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="M4" s="9">
         <v>1037695</v>
@@ -999,31 +1136,43 @@
       <c r="P4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="13" t="s">
-        <v>26</v>
+      <c r="Q4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="14">
+        <v>44029</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="D5" s="9">
         <v>993548536</v>
       </c>
       <c r="E5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>22</v>
@@ -1033,10 +1182,10 @@
         <v>244</v>
       </c>
       <c r="K5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="M5" s="9">
         <v>1037648</v>
@@ -1048,14 +1197,26 @@
         <v>42209</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>26</v>
+        <v>50</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="14">
+        <v>44036</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AA1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1">
     <cfRule type="duplicateValues" dxfId="13" priority="6"/>
     <cfRule type="duplicateValues" dxfId="12" priority="7"/>
@@ -1068,14 +1229,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B5">
     <cfRule type="duplicateValues" dxfId="9" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B5">
     <cfRule type="duplicateValues" dxfId="8" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E5">
-    <cfRule type="containsBlanks" dxfId="7" priority="14" stopIfTrue="1">
-      <formula>LEN(TRIM(E2))=0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C5 E2:I5">
     <cfRule type="iconSet" priority="15">
@@ -1084,6 +1238,11 @@
         <cfvo type="percent" val="33"/>
         <cfvo type="percent" val="67"/>
       </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E5">
+    <cfRule type="containsBlanks" dxfId="7" priority="14" stopIfTrue="1">
+      <formula>LEN(TRIM(E2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J5">
@@ -1097,15 +1256,11 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M5">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M5">
     <cfRule type="duplicateValues" dxfId="2" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N5">
-    <cfRule type="duplicateValues" dxfId="1" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N5">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="13"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>